<commit_message>
Add file THongTinHocSinh.xlsx, ImportStudent.php, ExportStudent.php
</commit_message>
<xml_diff>
--- a/PHPExcel/ExportData.xlsx
+++ b/PHPExcel/ExportData.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="10A1" sheetId="1" r:id="rId4"/>
+    <sheet name="Lop10A1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
@@ -17,43 +17,43 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
-    <t>Họ tên</t>
-  </si>
-  <si>
-    <t>Toán</t>
-  </si>
-  <si>
-    <t>Lý</t>
-  </si>
-  <si>
-    <t>Hóa</t>
-  </si>
-  <si>
-    <t>Ngô Trần Anh</t>
-  </si>
-  <si>
-    <t>Nguyễn Văn Vũ</t>
-  </si>
-  <si>
-    <t>Nguyễn Thanh Lam</t>
-  </si>
-  <si>
-    <t>Lê Hoàng Bảo Châu</t>
-  </si>
-  <si>
-    <t>Bùi Sỹ Khiên</t>
-  </si>
-  <si>
-    <t>Nguyễn Trung Hiếu</t>
-  </si>
-  <si>
-    <t>Lê Ngọc Sơn</t>
-  </si>
-  <si>
-    <t>Nguyễn Thu Thảo</t>
-  </si>
-  <si>
-    <t>Nguyễn Thành Danh</t>
+    <t>Họ và tên</t>
+  </si>
+  <si>
+    <t>Ngày Sinh</t>
+  </si>
+  <si>
+    <t>Giới Tính</t>
+  </si>
+  <si>
+    <t>Địa Chỉ</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn An</t>
+  </si>
+  <si>
+    <t>1990-04-24</t>
+  </si>
+  <si>
+    <t>243 Khuất Duy Tiến-Thanh Xuân-Hà Nội</t>
+  </si>
+  <si>
+    <t>Nguyễn Thi Thạch Anh</t>
+  </si>
+  <si>
+    <t>1990-07-18</t>
+  </si>
+  <si>
+    <t>Ba Vì-Hà Tây</t>
+  </si>
+  <si>
+    <t>Cao Quyết Thắng</t>
+  </si>
+  <si>
+    <t>1990-03-23</t>
+  </si>
+  <si>
+    <t>Tây Hòa-Phú Yên</t>
   </si>
 </sst>
 </file>
@@ -392,7 +392,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -418,140 +418,42 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>8.5</v>
+      <c r="B2" t="s">
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>8</v>
-      </c>
-      <c r="D2">
-        <v>9.2</v>
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
         <v>7</v>
       </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
       <c r="C3">
-        <v>6.8</v>
-      </c>
-      <c r="D3">
-        <v>8.7</v>
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>8.1</v>
-      </c>
-      <c r="C5">
-        <v>8.6</v>
-      </c>
-      <c r="D5">
-        <v>8.7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>9.5</v>
-      </c>
-      <c r="C6">
-        <v>9.2</v>
-      </c>
-      <c r="D6">
-        <v>8.8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>7</v>
-      </c>
-      <c r="C7">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>9.1</v>
-      </c>
-      <c r="C8">
-        <v>9</v>
-      </c>
-      <c r="D8">
-        <v>8.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <v>9</v>
-      </c>
-      <c r="C9">
-        <v>8</v>
-      </c>
-      <c r="D9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10">
-        <v>8.7</v>
-      </c>
-      <c r="C10">
-        <v>8.6</v>
-      </c>
-      <c r="D10">
-        <v>8.7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
-      </c>
-      <c r="B11">
-        <v>8.8</v>
-      </c>
-      <c r="C11">
-        <v>8</v>
-      </c>
-      <c r="D11">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>